<commit_message>
Currency changes between dates sheet implementation
</commit_message>
<xml_diff>
--- a/src/Controllers/Sheet/outputs/report-yesterday-today.xlsx
+++ b/src/Controllers/Sheet/outputs/report-yesterday-today.xlsx
@@ -70,13 +70,19 @@
     <t xml:space="preserve">Valor hoje (04/11/2021)</t>
   </si>
   <si>
-    <t xml:space="preserve">Dólar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Diminuiu 1.41%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">21:57</t>
+    <t xml:space="preserve">Iene</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JPY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">¥</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diminuiu 1.20%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">21:59</t>
   </si>
 </sst>
 </file>
@@ -571,19 +577,19 @@
         <v>12</v>
       </c>
       <c r="B2" t="s" s="5">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="C2" t="s" s="8">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="D2" s="5">
-        <v>5.68</v>
+        <v>0.0498</v>
       </c>
       <c r="E2" s="5">
-        <v>5.6</v>
+        <v>0.0492</v>
       </c>
       <c r="F2" t="s" s="8">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -611,7 +617,7 @@
       <c r="D5" s="5"/>
       <c r="E5" s="8"/>
       <c r="F5" t="s" s="12">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
baseURL fixed for report generation request
</commit_message>
<xml_diff>
--- a/src/Controllers/Sheet/outputs/report-yesterday-today.xlsx
+++ b/src/Controllers/Sheet/outputs/report-yesterday-today.xlsx
@@ -70,19 +70,13 @@
     <t xml:space="preserve">Valor hoje (04/11/2021)</t>
   </si>
   <si>
-    <t xml:space="preserve">Iene</t>
-  </si>
-  <si>
-    <t xml:space="preserve">JPY</t>
-  </si>
-  <si>
-    <t xml:space="preserve">¥</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Diminuiu 1.20%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">21:59</t>
+    <t xml:space="preserve">Dólar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diminuiu 1.41%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">22:08</t>
   </si>
 </sst>
 </file>
@@ -577,19 +571,19 @@
         <v>12</v>
       </c>
       <c r="B2" t="s" s="5">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s" s="8">
+        <v>8</v>
+      </c>
+      <c r="D2" s="5">
+        <v>5.68</v>
+      </c>
+      <c r="E2" s="5">
+        <v>5.6</v>
+      </c>
+      <c r="F2" t="s" s="8">
         <v>13</v>
-      </c>
-      <c r="C2" t="s" s="8">
-        <v>14</v>
-      </c>
-      <c r="D2" s="5">
-        <v>0.0498</v>
-      </c>
-      <c r="E2" s="5">
-        <v>0.0492</v>
-      </c>
-      <c r="F2" t="s" s="8">
-        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -617,7 +611,7 @@
       <c r="D5" s="5"/>
       <c r="E5" s="8"/>
       <c r="F5" t="s" s="12">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Create new currency behaviour simplified
</commit_message>
<xml_diff>
--- a/src/Controllers/Sheet/outputs/report-yesterday-today.xlsx
+++ b/src/Controllers/Sheet/outputs/report-yesterday-today.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\victo\Documents\Victor\currency_api\src\Controllers\Sheet\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\victo\Documents\Victor\currency_api\src\Controllers\Sheet\outputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B487441-F9BF-4CA6-9C74-E9257C93478E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C64010BC-027B-4D98-88D6-2BDAAF8432F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{D9CDE337-A4A4-4202-BDB0-1B9F047ECC56}" activeTab="0"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{D9CDE337-A4A4-4202-BDB0-1B9F047ECC56}"/>
   </bookViews>
   <sheets>
     <sheet name="Cotações" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Moeda</t>
   </si>
@@ -46,47 +46,38 @@
     <t>Resultado</t>
   </si>
   <si>
-    <t>Dolar</t>
-  </si>
-  <si>
-    <t>USD</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Valor ontem (01/11/2021)</t>
-  </si>
-  <si>
-    <t>Valor hoje (02/11/2021)</t>
-  </si>
-  <si>
-    <t>$</t>
-  </si>
-  <si>
     <t>Símbolo</t>
   </si>
   <si>
-    <t xml:space="preserve">Valor ontem (01/11/2021)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Valor hoje (04/11/2021)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dólar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Diminuiu 1.41%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">22:08</t>
+    <t>Valor ontem (11/11/2021)</t>
+  </si>
+  <si>
+    <t>Valor hoje (11/11/2021)</t>
+  </si>
+  <si>
+    <t>Coroa Norueguesa</t>
+  </si>
+  <si>
+    <t>NOK</t>
+  </si>
+  <si>
+    <t>kr</t>
+  </si>
+  <si>
+    <t>Nenhuma mudança</t>
+  </si>
+  <si>
+    <t>21:28</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts>
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;R$&quot;\ #,##0.00"/>
   </numFmts>
-  <fonts x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -116,7 +107,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills>
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -136,7 +127,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders>
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -148,7 +139,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs>
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -531,11 +522,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CE66C2D-1CA9-406C-B2E0-06F7FFA9C030}">
-  <sheetPr/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -547,43 +536,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" t="s" s="2">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="2">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s" s="9">
+      <c r="C1" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="D1" t="s" s="2">
+      <c r="D2" s="5">
+        <v>0.62</v>
+      </c>
+      <c r="E2" s="5">
+        <v>0.62</v>
+      </c>
+      <c r="F2" s="8" t="s">
         <v>10</v>
-      </c>
-      <c r="E1" t="s" s="3">
-        <v>11</v>
-      </c>
-      <c r="F1" t="s" s="9">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s" s="1">
-        <v>12</v>
-      </c>
-      <c r="B2" t="s" s="5">
-        <v>5</v>
-      </c>
-      <c r="C2" t="s" s="8">
-        <v>8</v>
-      </c>
-      <c r="D2" s="5">
-        <v>5.68</v>
-      </c>
-      <c r="E2" s="5">
-        <v>5.6</v>
-      </c>
-      <c r="F2" t="s" s="8">
-        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -600,7 +589,7 @@
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
       <c r="E4" s="8"/>
-      <c r="F4" t="s" s="4">
+      <c r="F4" s="4" t="s">
         <v>2</v>
       </c>
     </row>
@@ -610,8 +599,8 @@
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
       <c r="E5" s="8"/>
-      <c r="F5" t="s" s="12">
-        <v>14</v>
+      <c r="F5" s="12" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>